<commit_message>
polarised capacitors are not 0805 anymore
they are now elco capacitors (pcb image still needs updated)
</commit_message>
<xml_diff>
--- a/Info/BOM.xlsx
+++ b/Info/BOM.xlsx
@@ -90,7 +90,7 @@
     <t xml:space="preserve">CL21 Series 0805</t>
   </si>
   <si>
-    <t xml:space="preserve">SMD 0805 Ceramic Capacitor</t>
+    <t xml:space="preserve">SMD 0805 Ceramic Capacitor (Not Polarised)</t>
   </si>
   <si>
     <t xml:space="preserve">C7, C10, C13, C14</t>
@@ -111,7 +111,7 @@
     <t>TAJR684K016RNJ</t>
   </si>
   <si>
-    <t xml:space="preserve">SMD 0805 Tantalum Capacitor</t>
+    <t xml:space="preserve">SMD Elco Capacitor (Polarised)</t>
   </si>
   <si>
     <t xml:space="preserve">C8–C12, C15–C25</t>
@@ -509,12 +509,9 @@
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="2" fillId="3" borderId="1" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="4" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -538,11 +535,17 @@
     <xf fontId="0" fillId="5" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf fontId="0" fillId="5" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="0" fillId="5" borderId="5" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="6" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1075,762 +1078,762 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>2</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>2</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>4</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="9"/>
+      <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>2</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>2</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>4</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="4">
+      <c r="C9" s="5"/>
+      <c r="D9" s="3">
         <v>1</v>
       </c>
       <c r="E9" s="12"/>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="4">
+      <c r="C10" s="5"/>
+      <c r="D10" s="3">
         <v>1</v>
       </c>
       <c r="E10" s="12"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="4">
+      <c r="C11" s="5"/>
+      <c r="D11" s="3">
         <v>1</v>
       </c>
       <c r="E11" s="12"/>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="4">
+      <c r="C12" s="5"/>
+      <c r="D12" s="3">
         <v>1</v>
       </c>
       <c r="E12" s="12"/>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>15</v>
       </c>
       <c r="E13" s="12"/>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" s="13"/>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="4">
+      <c r="C14" s="5"/>
+      <c r="D14" s="3">
         <v>4</v>
       </c>
       <c r="E14" s="12"/>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="5" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="4">
+      <c r="C15" s="5"/>
+      <c r="D15" s="3">
         <v>6</v>
       </c>
       <c r="E15" s="12"/>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="5" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="4">
+      <c r="C16" s="5"/>
+      <c r="D16" s="3">
         <v>5</v>
       </c>
-      <c r="E16" s="11"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="4">
-        <v>1</v>
-      </c>
-      <c r="E17" s="4"/>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3"/>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="4">
-        <v>1</v>
-      </c>
-      <c r="E18" s="4"/>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="3">
         <v>2</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="4">
-        <v>1</v>
-      </c>
-      <c r="E20" s="4"/>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="4">
-        <v>1</v>
-      </c>
-      <c r="E21" s="4"/>
+      <c r="D21" s="3">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <v>4</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="4">
-        <v>1</v>
-      </c>
-      <c r="E23" s="4"/>
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3"/>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="3">
         <v>2</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="3">
         <v>11</v>
       </c>
-      <c r="E25" s="4"/>
+      <c r="E25" s="3"/>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="6">
         <v>9</v>
       </c>
-      <c r="E26" s="7"/>
+      <c r="E26" s="6"/>
     </row>
     <row r="27" ht="14.25">
       <c r="A27" s="13"/>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="3">
         <v>3</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="6" t="s">
+      <c r="A28" s="9"/>
+      <c r="B28" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="4">
-        <v>1</v>
-      </c>
-      <c r="E28" s="7" t="s">
+      <c r="D28" s="3">
+        <v>1</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="10"/>
-      <c r="B29" s="6" t="s">
+      <c r="A29" s="9"/>
+      <c r="B29" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="4">
-        <v>1</v>
-      </c>
-      <c r="E29" s="7" t="s">
+      <c r="D29" s="3">
+        <v>1</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="6" t="s">
+      <c r="A30" s="9"/>
+      <c r="B30" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="3">
         <v>4</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="31" ht="14.25">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D31" s="15">
         <v>39</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="32" ht="14.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="6" t="s">
+      <c r="A32" s="9"/>
+      <c r="B32" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="4">
+      <c r="C32" s="5"/>
+      <c r="D32" s="3">
         <v>1</v>
       </c>
       <c r="E32" s="12"/>
     </row>
     <row r="33" ht="14.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="6" t="s">
+      <c r="A33" s="9"/>
+      <c r="B33" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="4">
+      <c r="C33" s="5"/>
+      <c r="D33" s="3">
         <v>1</v>
       </c>
       <c r="E33" s="12"/>
     </row>
     <row r="34" ht="14.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="6" t="s">
+      <c r="A34" s="9"/>
+      <c r="B34" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="4">
+      <c r="C34" s="5"/>
+      <c r="D34" s="3">
         <v>1</v>
       </c>
       <c r="E34" s="12"/>
     </row>
     <row r="35" ht="14.25">
-      <c r="A35" s="10"/>
-      <c r="B35" s="6" t="s">
+      <c r="A35" s="9"/>
+      <c r="B35" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="4">
+      <c r="C35" s="5"/>
+      <c r="D35" s="3">
         <v>1</v>
       </c>
       <c r="E35" s="12"/>
     </row>
     <row r="36" ht="14.25">
-      <c r="A36" s="10"/>
-      <c r="B36" s="6" t="s">
+      <c r="A36" s="9"/>
+      <c r="B36" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="4">
+      <c r="C36" s="5"/>
+      <c r="D36" s="3">
         <v>1</v>
       </c>
       <c r="E36" s="12"/>
     </row>
     <row r="37" ht="14.25">
-      <c r="A37" s="10"/>
-      <c r="B37" s="6" t="s">
+      <c r="A37" s="9"/>
+      <c r="B37" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="4">
+      <c r="C37" s="5"/>
+      <c r="D37" s="3">
         <v>9</v>
       </c>
       <c r="E37" s="12"/>
     </row>
     <row r="38" ht="14.25">
-      <c r="A38" s="10"/>
-      <c r="B38" s="6" t="s">
+      <c r="A38" s="9"/>
+      <c r="B38" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="4">
+      <c r="C38" s="5"/>
+      <c r="D38" s="3">
         <v>4</v>
       </c>
       <c r="E38" s="12"/>
     </row>
     <row r="39" ht="14.25">
-      <c r="A39" s="10"/>
-      <c r="B39" s="6" t="s">
+      <c r="A39" s="9"/>
+      <c r="B39" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="4">
+      <c r="C39" s="5"/>
+      <c r="D39" s="3">
         <v>2</v>
       </c>
       <c r="E39" s="12"/>
     </row>
     <row r="40" ht="14.25">
-      <c r="A40" s="10"/>
-      <c r="B40" s="6" t="s">
+      <c r="A40" s="9"/>
+      <c r="B40" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="4">
+      <c r="C40" s="5"/>
+      <c r="D40" s="3">
         <v>1</v>
       </c>
       <c r="E40" s="12"/>
     </row>
     <row r="41" ht="14.25">
-      <c r="A41" s="10"/>
-      <c r="B41" s="6" t="s">
+      <c r="A41" s="9"/>
+      <c r="B41" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="4">
+      <c r="C41" s="5"/>
+      <c r="D41" s="3">
         <v>2</v>
       </c>
       <c r="E41" s="12"/>
     </row>
     <row r="42" ht="14.25">
-      <c r="A42" s="10"/>
-      <c r="B42" s="6" t="s">
+      <c r="A42" s="9"/>
+      <c r="B42" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="4">
+      <c r="C42" s="5"/>
+      <c r="D42" s="3">
         <v>3</v>
       </c>
       <c r="E42" s="12"/>
     </row>
     <row r="43" ht="14.25">
-      <c r="A43" s="10"/>
-      <c r="B43" s="6" t="s">
+      <c r="A43" s="9"/>
+      <c r="B43" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="4">
+      <c r="C43" s="5"/>
+      <c r="D43" s="3">
         <v>6</v>
       </c>
       <c r="E43" s="12"/>
     </row>
     <row r="44" ht="14.25">
-      <c r="A44" s="10"/>
-      <c r="B44" s="6" t="s">
+      <c r="A44" s="9"/>
+      <c r="B44" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="4">
+      <c r="C44" s="5"/>
+      <c r="D44" s="3">
         <v>1</v>
       </c>
       <c r="E44" s="12"/>
     </row>
     <row r="45" ht="14.25">
-      <c r="A45" s="10"/>
-      <c r="B45" s="6" t="s">
+      <c r="A45" s="9"/>
+      <c r="B45" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="4">
+      <c r="C45" s="5"/>
+      <c r="D45" s="3">
         <v>1</v>
       </c>
       <c r="E45" s="12"/>
     </row>
     <row r="46" ht="14.25">
-      <c r="A46" s="10"/>
-      <c r="B46" s="6" t="s">
+      <c r="A46" s="9"/>
+      <c r="B46" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="4">
+      <c r="C46" s="5"/>
+      <c r="D46" s="3">
         <v>1</v>
       </c>
       <c r="E46" s="12"/>
     </row>
     <row r="47" ht="14.25">
-      <c r="A47" s="10"/>
-      <c r="B47" s="6" t="s">
+      <c r="A47" s="9"/>
+      <c r="B47" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="4">
+      <c r="C47" s="5"/>
+      <c r="D47" s="3">
         <v>1</v>
       </c>
       <c r="E47" s="12"/>
     </row>
     <row r="48" ht="14.25">
-      <c r="A48" s="10"/>
-      <c r="B48" s="6" t="s">
+      <c r="A48" s="9"/>
+      <c r="B48" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="4">
+      <c r="C48" s="5"/>
+      <c r="D48" s="3">
         <v>1</v>
       </c>
       <c r="E48" s="12"/>
     </row>
     <row r="49" ht="14.25">
-      <c r="A49" s="10"/>
-      <c r="B49" s="6" t="s">
+      <c r="A49" s="9"/>
+      <c r="B49" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C49" s="6"/>
-      <c r="D49" s="4">
+      <c r="C49" s="5"/>
+      <c r="D49" s="3">
         <v>1</v>
       </c>
       <c r="E49" s="12"/>
     </row>
     <row r="50" ht="14.25">
-      <c r="A50" s="10"/>
-      <c r="B50" s="6" t="s">
+      <c r="A50" s="9"/>
+      <c r="B50" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C50" s="6"/>
-      <c r="D50" s="4">
-        <v>1</v>
-      </c>
-      <c r="E50" s="11"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="3">
+        <v>1</v>
+      </c>
+      <c r="E50" s="10"/>
     </row>
     <row r="51" ht="14.25">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C51" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D51" s="4">
+      <c r="D51" s="3">
         <v>4</v>
       </c>
-      <c r="E51" s="4"/>
+      <c r="E51" s="3"/>
     </row>
     <row r="52" ht="14.25">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D52" s="4">
-        <v>1</v>
-      </c>
-      <c r="E52" s="4"/>
+      <c r="D52" s="3">
+        <v>1</v>
+      </c>
+      <c r="E52" s="3"/>
     </row>
     <row r="53" ht="14.25">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C53" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D53" s="4">
-        <v>1</v>
-      </c>
-      <c r="E53" s="4"/>
+      <c r="D53" s="3">
+        <v>1</v>
+      </c>
+      <c r="E53" s="3"/>
     </row>
     <row r="54" ht="14.25">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D54" s="4">
+      <c r="D54" s="3">
         <v>4</v>
       </c>
-      <c r="E54" s="4"/>
+      <c r="E54" s="3"/>
     </row>
     <row r="55" ht="14.25">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D55" s="4">
-        <v>1</v>
-      </c>
-      <c r="E55" s="4"/>
+      <c r="D55" s="3">
+        <v>1</v>
+      </c>
+      <c r="E55" s="3"/>
     </row>
     <row r="56" ht="14.25">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C56" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D56" s="4">
-        <v>1</v>
-      </c>
-      <c r="E56" s="4"/>
+      <c r="D56" s="3">
+        <v>1</v>
+      </c>
+      <c r="E56" s="3"/>
     </row>
     <row r="57" ht="14.25">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D57" s="4">
-        <v>1</v>
-      </c>
-      <c r="E57" s="4"/>
+      <c r="D57" s="3">
+        <v>1</v>
+      </c>
+      <c r="E57" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
final commit for PO
</commit_message>
<xml_diff>
--- a/Info/BOM.xlsx
+++ b/Info/BOM.xlsx
@@ -535,11 +535,11 @@
     <xf fontId="0" fillId="5" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf fontId="0" fillId="5" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="0" fillId="5" borderId="5" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="5" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="6" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1186,7 +1186,7 @@
       <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -1208,7 +1208,7 @@
       <c r="D9" s="3">
         <v>1</v>
       </c>
-      <c r="E9" s="11"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="9"/>
@@ -1219,7 +1219,7 @@
       <c r="D10" s="3">
         <v>1</v>
       </c>
-      <c r="E10" s="11"/>
+      <c r="E10" s="12"/>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" s="9"/>
@@ -1230,7 +1230,7 @@
       <c r="D11" s="3">
         <v>1</v>
       </c>
-      <c r="E11" s="11"/>
+      <c r="E11" s="12"/>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" s="9"/>
@@ -1241,10 +1241,10 @@
       <c r="D12" s="3">
         <v>1</v>
       </c>
-      <c r="E12" s="11"/>
+      <c r="E12" s="12"/>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -1256,7 +1256,7 @@
       <c r="D13" s="6">
         <v>15</v>
       </c>
-      <c r="E13" s="11"/>
+      <c r="E13" s="12"/>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" s="13"/>
@@ -1267,7 +1267,7 @@
       <c r="D14" s="3">
         <v>4</v>
       </c>
-      <c r="E14" s="11"/>
+      <c r="E14" s="12"/>
     </row>
     <row r="15" ht="14.25">
       <c r="A15" s="9"/>
@@ -1278,7 +1278,7 @@
       <c r="D15" s="3">
         <v>6</v>
       </c>
-      <c r="E15" s="11"/>
+      <c r="E15" s="12"/>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" s="9"/>
@@ -1527,7 +1527,7 @@
       <c r="D32" s="3">
         <v>1</v>
       </c>
-      <c r="E32" s="11"/>
+      <c r="E32" s="12"/>
     </row>
     <row r="33" ht="14.25">
       <c r="A33" s="9"/>
@@ -1538,7 +1538,7 @@
       <c r="D33" s="3">
         <v>1</v>
       </c>
-      <c r="E33" s="11"/>
+      <c r="E33" s="12"/>
     </row>
     <row r="34" ht="14.25">
       <c r="A34" s="9"/>
@@ -1549,7 +1549,7 @@
       <c r="D34" s="3">
         <v>1</v>
       </c>
-      <c r="E34" s="11"/>
+      <c r="E34" s="12"/>
     </row>
     <row r="35" ht="14.25">
       <c r="A35" s="9"/>
@@ -1560,7 +1560,7 @@
       <c r="D35" s="3">
         <v>1</v>
       </c>
-      <c r="E35" s="11"/>
+      <c r="E35" s="12"/>
     </row>
     <row r="36" ht="14.25">
       <c r="A36" s="9"/>
@@ -1571,7 +1571,7 @@
       <c r="D36" s="3">
         <v>1</v>
       </c>
-      <c r="E36" s="11"/>
+      <c r="E36" s="12"/>
     </row>
     <row r="37" ht="14.25">
       <c r="A37" s="9"/>
@@ -1582,7 +1582,7 @@
       <c r="D37" s="3">
         <v>9</v>
       </c>
-      <c r="E37" s="11"/>
+      <c r="E37" s="12"/>
     </row>
     <row r="38" ht="14.25">
       <c r="A38" s="9"/>
@@ -1593,7 +1593,7 @@
       <c r="D38" s="3">
         <v>4</v>
       </c>
-      <c r="E38" s="11"/>
+      <c r="E38" s="12"/>
     </row>
     <row r="39" ht="14.25">
       <c r="A39" s="9"/>
@@ -1604,7 +1604,7 @@
       <c r="D39" s="3">
         <v>2</v>
       </c>
-      <c r="E39" s="11"/>
+      <c r="E39" s="12"/>
     </row>
     <row r="40" ht="14.25">
       <c r="A40" s="9"/>
@@ -1615,7 +1615,7 @@
       <c r="D40" s="3">
         <v>1</v>
       </c>
-      <c r="E40" s="11"/>
+      <c r="E40" s="12"/>
     </row>
     <row r="41" ht="14.25">
       <c r="A41" s="9"/>
@@ -1626,7 +1626,7 @@
       <c r="D41" s="3">
         <v>2</v>
       </c>
-      <c r="E41" s="11"/>
+      <c r="E41" s="12"/>
     </row>
     <row r="42" ht="14.25">
       <c r="A42" s="9"/>
@@ -1637,7 +1637,7 @@
       <c r="D42" s="3">
         <v>3</v>
       </c>
-      <c r="E42" s="11"/>
+      <c r="E42" s="12"/>
     </row>
     <row r="43" ht="14.25">
       <c r="A43" s="9"/>
@@ -1648,7 +1648,7 @@
       <c r="D43" s="3">
         <v>6</v>
       </c>
-      <c r="E43" s="11"/>
+      <c r="E43" s="12"/>
     </row>
     <row r="44" ht="14.25">
       <c r="A44" s="9"/>
@@ -1659,7 +1659,7 @@
       <c r="D44" s="3">
         <v>1</v>
       </c>
-      <c r="E44" s="11"/>
+      <c r="E44" s="12"/>
     </row>
     <row r="45" ht="14.25">
       <c r="A45" s="9"/>
@@ -1670,7 +1670,7 @@
       <c r="D45" s="3">
         <v>1</v>
       </c>
-      <c r="E45" s="11"/>
+      <c r="E45" s="12"/>
     </row>
     <row r="46" ht="14.25">
       <c r="A46" s="9"/>
@@ -1681,7 +1681,7 @@
       <c r="D46" s="3">
         <v>1</v>
       </c>
-      <c r="E46" s="11"/>
+      <c r="E46" s="12"/>
     </row>
     <row r="47" ht="14.25">
       <c r="A47" s="9"/>
@@ -1692,7 +1692,7 @@
       <c r="D47" s="3">
         <v>1</v>
       </c>
-      <c r="E47" s="11"/>
+      <c r="E47" s="12"/>
     </row>
     <row r="48" ht="14.25">
       <c r="A48" s="9"/>
@@ -1703,7 +1703,7 @@
       <c r="D48" s="3">
         <v>1</v>
       </c>
-      <c r="E48" s="11"/>
+      <c r="E48" s="12"/>
     </row>
     <row r="49" ht="14.25">
       <c r="A49" s="9"/>
@@ -1714,7 +1714,7 @@
       <c r="D49" s="3">
         <v>1</v>
       </c>
-      <c r="E49" s="11"/>
+      <c r="E49" s="12"/>
     </row>
     <row r="50" ht="14.25">
       <c r="A50" s="9"/>

</xml_diff>